<commit_message>
Have got N responeses in wheat beaving, need further work on Miniralisation
</commit_message>
<xml_diff>
--- a/Simulations/Observations/Wheat/SoilDailyLayerMeans.xlsx
+++ b/Simulations/Observations/Wheat/SoilDailyLayerMeans.xlsx
@@ -502,11 +502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="392156888"/>
-        <c:axId val="392156496"/>
+        <c:axId val="209492936"/>
+        <c:axId val="209493320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="392156888"/>
+        <c:axId val="209492936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,12 +563,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392156496"/>
+        <c:crossAx val="209493320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="392156496"/>
+        <c:axId val="209493320"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -625,7 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392156888"/>
+        <c:crossAx val="209492936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -972,11 +972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="383554720"/>
-        <c:axId val="383557856"/>
+        <c:axId val="207408208"/>
+        <c:axId val="207408600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="383554720"/>
+        <c:axId val="207408208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,12 +1033,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383557856"/>
+        <c:crossAx val="207408600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="383557856"/>
+        <c:axId val="207408600"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1095,7 +1095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383554720"/>
+        <c:crossAx val="207408208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1442,11 +1442,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="305054280"/>
-        <c:axId val="383557072"/>
+        <c:axId val="207409384"/>
+        <c:axId val="207409776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="305054280"/>
+        <c:axId val="207409384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,12 +1503,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383557072"/>
+        <c:crossAx val="207409776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="383557072"/>
+        <c:axId val="207409776"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1565,7 +1565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="305054280"/>
+        <c:crossAx val="207409384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1908,11 +1908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="365176544"/>
-        <c:axId val="365175760"/>
+        <c:axId val="207410560"/>
+        <c:axId val="207410952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="365176544"/>
+        <c:axId val="207410560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,12 +1969,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365175760"/>
+        <c:crossAx val="207410952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="365175760"/>
+        <c:axId val="207410952"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2031,7 +2031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365176544"/>
+        <c:crossAx val="207410560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2374,11 +2374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="313043488"/>
-        <c:axId val="383556288"/>
+        <c:axId val="208981768"/>
+        <c:axId val="208982160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="313043488"/>
+        <c:axId val="208981768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2435,12 +2435,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383556288"/>
+        <c:crossAx val="208982160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="383556288"/>
+        <c:axId val="208982160"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2497,7 +2497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313043488"/>
+        <c:crossAx val="208981768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2840,11 +2840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="315774160"/>
-        <c:axId val="315777688"/>
+        <c:axId val="208982944"/>
+        <c:axId val="209565640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="315774160"/>
+        <c:axId val="208982944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,12 +2901,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315777688"/>
+        <c:crossAx val="209565640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="315777688"/>
+        <c:axId val="209565640"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2963,7 +2963,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315774160"/>
+        <c:crossAx val="208982944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26345,17 +26345,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="AF1:AK1"/>
-    <mergeCell ref="Z1:AE1"/>
-    <mergeCell ref="T1:Y1"/>
-    <mergeCell ref="N1:S1"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="K2:M2"/>
     <mergeCell ref="AO2:AQ2"/>
     <mergeCell ref="AR1:AW1"/>
     <mergeCell ref="H1:M1"/>
@@ -26369,6 +26358,17 @@
     <mergeCell ref="AU2:AW2"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="AR2:AT2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -59966,10 +59966,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:S28"/>
+  <dimension ref="A3:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -59977,12 +59977,12 @@
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -59990,7 +59990,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0</v>
       </c>
@@ -60010,7 +60010,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -60030,7 +60030,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -60088,8 +60088,12 @@
         <f>MAX(Data!F10:F135)</f>
         <v>0.33353750000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U7">
+        <f>MAX(C7,F7,I7,)</f>
+        <v>0.31093749999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>30</v>
       </c>
@@ -60147,8 +60151,12 @@
         <f>MAX(Data!R11:R136)</f>
         <v>0.31524999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U8">
+        <f t="shared" ref="U8:U13" si="0">MAX(C8,F8,I8,)</f>
+        <v>0.28869374999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>60</v>
       </c>
@@ -60206,8 +60214,12 @@
         <f>MAX(Data!V12:V137)</f>
         <v>0.29339999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>0.29951250000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>90</v>
       </c>
@@ -60265,8 +60277,12 @@
         <f>MAX(Data!AD13:AD138)</f>
         <v>0.24116874999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>0.27823749999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>120</v>
       </c>
@@ -60324,8 +60340,12 @@
         <f>MAX(Data!AJ14:AJ139)</f>
         <v>0.27706249999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>0.29306874999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>150</v>
       </c>
@@ -60383,8 +60403,12 @@
         <f>MAX(Data!AP15:AP140)</f>
         <v>0.34839999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>0.34584999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>180</v>
       </c>
@@ -60441,6 +60465,10 @@
       <c r="S13">
         <f>MAX(Data!AU16:AU141)</f>
         <v>0.25491249999999999</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>0.30260624999999997</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>